<commit_message>
Basic login in  and logout functionality in navbar
</commit_message>
<xml_diff>
--- a/Accounting App Planning.xlsx
+++ b/Accounting App Planning.xlsx
@@ -5,21 +5,22 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Louise\Documents\GitHub\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Louise\Documents\GitHub\AccountingApp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0C4A9E0-8F66-4DEE-9D1A-CA40EB469E07}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{912DEAB8-3CB0-4A9C-913D-7F819AA10B98}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7920" activeTab="1" xr2:uid="{87DFCFEA-2F07-4D1A-89B8-93DFC4EF050B}"/>
   </bookViews>
   <sheets>
     <sheet name="Tables" sheetId="1" r:id="rId1"/>
-    <sheet name="Transactions" sheetId="7" r:id="rId2"/>
-    <sheet name="Debtors" sheetId="5" r:id="rId3"/>
-    <sheet name="Creditors" sheetId="6" r:id="rId4"/>
-    <sheet name="Accounts" sheetId="4" r:id="rId5"/>
-    <sheet name="Type" sheetId="3" r:id="rId6"/>
-    <sheet name="Users" sheetId="2" r:id="rId7"/>
+    <sheet name="CashBook" sheetId="7" r:id="rId2"/>
+    <sheet name="Journal" sheetId="8" r:id="rId3"/>
+    <sheet name="Debtors" sheetId="5" r:id="rId4"/>
+    <sheet name="Creditors" sheetId="6" r:id="rId5"/>
+    <sheet name="Accounts" sheetId="4" r:id="rId6"/>
+    <sheet name="Type" sheetId="3" r:id="rId7"/>
+    <sheet name="Users" sheetId="2" r:id="rId8"/>
   </sheets>
   <calcPr calcId="179021"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="65">
   <si>
     <t>Tables</t>
   </si>
@@ -182,9 +183,6 @@
     <t>Payment Received</t>
   </si>
   <si>
-    <t>Medical Expenses</t>
-  </si>
-  <si>
     <t>25.10.2018</t>
   </si>
   <si>
@@ -198,6 +196,42 @@
   </si>
   <si>
     <t>Payment made</t>
+  </si>
+  <si>
+    <t>AccountName</t>
+  </si>
+  <si>
+    <t>GLTypeId</t>
+  </si>
+  <si>
+    <t>AccountType</t>
+  </si>
+  <si>
+    <t>Trusave</t>
+  </si>
+  <si>
+    <t>Home Loan</t>
+  </si>
+  <si>
+    <t>AccountTypeId</t>
+  </si>
+  <si>
+    <t>Descr</t>
+  </si>
+  <si>
+    <t>Medical Aid</t>
+  </si>
+  <si>
+    <t>Debtor/CreditorId</t>
+  </si>
+  <si>
+    <t>Absa</t>
+  </si>
+  <si>
+    <t>Contra Account</t>
+  </si>
+  <si>
+    <t>Bank Acc</t>
   </si>
 </sst>
 </file>
@@ -207,7 +241,7 @@
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_-&quot;R&quot;* #,##0.00_-;\-&quot;R&quot;* #,##0.00_-;_-&quot;R&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -215,13 +249,33 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -236,9 +290,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -556,7 +613,7 @@
   <dimension ref="A1:A8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -606,10 +663,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79F3F73F-D9F7-4B2F-A93D-F7A699778583}">
-  <dimension ref="A1:H13"/>
+  <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="G19" sqref="A19:G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -619,6 +676,7 @@
     <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -804,61 +862,21 @@
         <v>8000</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>5</v>
-      </c>
-      <c r="B10" t="s">
-        <v>48</v>
-      </c>
-      <c r="C10" t="s">
-        <v>49</v>
-      </c>
-      <c r="D10" t="s">
-        <v>37</v>
-      </c>
-      <c r="E10" t="s">
-        <v>50</v>
-      </c>
-      <c r="F10" s="1">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>5</v>
-      </c>
-      <c r="B11" t="s">
-        <v>51</v>
-      </c>
-      <c r="C11" t="s">
-        <v>49</v>
-      </c>
-      <c r="D11" t="s">
-        <v>42</v>
-      </c>
-      <c r="E11" t="s">
-        <v>50</v>
-      </c>
-      <c r="F11" s="1">
-        <v>2000</v>
-      </c>
-    </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>6</v>
       </c>
       <c r="B12" t="s">
+        <v>50</v>
+      </c>
+      <c r="C12" t="s">
         <v>51</v>
-      </c>
-      <c r="C12" t="s">
-        <v>52</v>
       </c>
       <c r="D12" t="s">
         <v>37</v>
       </c>
       <c r="E12" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F12" s="1">
         <v>1500</v>
@@ -872,16 +890,165 @@
         <v>38</v>
       </c>
       <c r="C13" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D13" t="s">
         <v>42</v>
       </c>
       <c r="E13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F13" s="1">
         <v>1500</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>5</v>
+      </c>
+      <c r="B18" t="s">
+        <v>39</v>
+      </c>
+      <c r="C18" t="s">
+        <v>35</v>
+      </c>
+      <c r="D18" t="s">
+        <v>34</v>
+      </c>
+      <c r="E18" t="s">
+        <v>11</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G18" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>1</v>
+      </c>
+      <c r="B19" t="s">
+        <v>38</v>
+      </c>
+      <c r="C19" t="s">
+        <v>41</v>
+      </c>
+      <c r="D19" t="s">
+        <v>37</v>
+      </c>
+      <c r="E19" t="s">
+        <v>21</v>
+      </c>
+      <c r="F19" s="1">
+        <v>75000</v>
+      </c>
+      <c r="G19" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>2</v>
+      </c>
+      <c r="B20" t="s">
+        <v>22</v>
+      </c>
+      <c r="C20" t="s">
+        <v>41</v>
+      </c>
+      <c r="D20" t="s">
+        <v>37</v>
+      </c>
+      <c r="E20" t="s">
+        <v>22</v>
+      </c>
+      <c r="F20" s="1">
+        <v>8000</v>
+      </c>
+      <c r="G20" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>3</v>
+      </c>
+      <c r="B21" t="s">
+        <v>44</v>
+      </c>
+      <c r="C21" t="s">
+        <v>41</v>
+      </c>
+      <c r="D21" t="s">
+        <v>37</v>
+      </c>
+      <c r="E21" t="s">
+        <v>45</v>
+      </c>
+      <c r="F21" s="1">
+        <v>8000</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>3</v>
+      </c>
+      <c r="B22" t="s">
+        <v>43</v>
+      </c>
+      <c r="C22" t="s">
+        <v>41</v>
+      </c>
+      <c r="D22" t="s">
+        <v>42</v>
+      </c>
+      <c r="E22" t="s">
+        <v>45</v>
+      </c>
+      <c r="F22" s="1">
+        <v>8000</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>4</v>
+      </c>
+      <c r="B23" t="s">
+        <v>38</v>
+      </c>
+      <c r="C23" t="s">
+        <v>46</v>
+      </c>
+      <c r="D23" t="s">
+        <v>37</v>
+      </c>
+      <c r="E23" t="s">
+        <v>47</v>
+      </c>
+      <c r="F23" s="1">
+        <v>8000</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>4</v>
+      </c>
+      <c r="B24" t="s">
+        <v>44</v>
+      </c>
+      <c r="C24" t="s">
+        <v>46</v>
+      </c>
+      <c r="D24" t="s">
+        <v>42</v>
+      </c>
+      <c r="E24" t="s">
+        <v>47</v>
+      </c>
+      <c r="F24" s="1">
+        <v>8000</v>
       </c>
     </row>
   </sheetData>
@@ -891,11 +1058,71 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{795508EF-A9E5-4557-BBD9-5B3FCB0F605F}">
-  <dimension ref="A1:B3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF958751-2910-4EF5-BAC8-9BEB2CE5B02A}">
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="2.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F2" s="1">
+        <v>2000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{795508EF-A9E5-4557-BBD9-5B3FCB0F605F}">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -903,7 +1130,7 @@
     <col min="2" max="2" width="20.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>18</v>
       </c>
@@ -911,20 +1138,31 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C2">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>30</v>
+      </c>
+      <c r="C3">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C4">
+        <v>1000</v>
       </c>
     </row>
   </sheetData>
@@ -932,12 +1170,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A1F12B1-9D57-4B6C-B32D-5F67BC6114C0}">
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -982,17 +1220,25 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDBAC260-C536-435A-8E99-0D8EB7825AD9}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:R23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="10" max="10" width="2.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.85546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -1006,7 +1252,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1020,7 +1266,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1034,7 +1280,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1047,8 +1293,11 @@
       <c r="D4">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1062,7 +1311,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1076,7 +1325,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1090,17 +1339,190 @@
         <v>1</v>
       </c>
     </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="J16" t="s">
+        <v>5</v>
+      </c>
+      <c r="K16" t="s">
+        <v>53</v>
+      </c>
+      <c r="L16" t="s">
+        <v>54</v>
+      </c>
+      <c r="M16" t="s">
+        <v>55</v>
+      </c>
+      <c r="N16" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q16" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="R16" s="4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="17" spans="10:18" x14ac:dyDescent="0.25">
+      <c r="J17">
+        <v>1</v>
+      </c>
+      <c r="K17" t="s">
+        <v>21</v>
+      </c>
+      <c r="L17" t="s">
+        <v>12</v>
+      </c>
+      <c r="M17" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="N17">
+        <v>1</v>
+      </c>
+      <c r="Q17">
+        <v>1</v>
+      </c>
+      <c r="R17" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="18" spans="10:18" x14ac:dyDescent="0.25">
+      <c r="J18">
+        <v>2</v>
+      </c>
+      <c r="K18" t="s">
+        <v>22</v>
+      </c>
+      <c r="L18" t="s">
+        <v>13</v>
+      </c>
+      <c r="M18" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="N18">
+        <v>1</v>
+      </c>
+      <c r="Q18">
+        <v>2</v>
+      </c>
+      <c r="R18" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19" spans="10:18" x14ac:dyDescent="0.25">
+      <c r="J19">
+        <v>3</v>
+      </c>
+      <c r="K19" t="s">
+        <v>44</v>
+      </c>
+      <c r="L19" t="s">
+        <v>23</v>
+      </c>
+      <c r="M19" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="N19">
+        <v>1</v>
+      </c>
+      <c r="Q19">
+        <v>3</v>
+      </c>
+      <c r="R19" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="20" spans="10:18" x14ac:dyDescent="0.25">
+      <c r="J20">
+        <v>4</v>
+      </c>
+      <c r="K20" t="s">
+        <v>56</v>
+      </c>
+      <c r="L20" t="s">
+        <v>23</v>
+      </c>
+      <c r="M20" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="N20">
+        <v>1</v>
+      </c>
+      <c r="Q20">
+        <v>4</v>
+      </c>
+      <c r="R20" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="21" spans="10:18" x14ac:dyDescent="0.25">
+      <c r="J21">
+        <v>5</v>
+      </c>
+      <c r="K21" t="s">
+        <v>50</v>
+      </c>
+      <c r="L21" t="s">
+        <v>26</v>
+      </c>
+      <c r="M21" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="N21">
+        <v>1</v>
+      </c>
+      <c r="Q21">
+        <v>5</v>
+      </c>
+      <c r="R21" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="22" spans="10:18" x14ac:dyDescent="0.25">
+      <c r="J22">
+        <v>6</v>
+      </c>
+      <c r="K22" t="s">
+        <v>57</v>
+      </c>
+      <c r="L22" t="s">
+        <v>26</v>
+      </c>
+      <c r="M22" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="N22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="10:18" x14ac:dyDescent="0.25">
+      <c r="J23">
+        <v>7</v>
+      </c>
+      <c r="K23" t="s">
+        <v>60</v>
+      </c>
+      <c r="L23" t="s">
+        <v>13</v>
+      </c>
+      <c r="M23" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="N23">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F992D269-6C39-4350-AEE8-3CE74A1271D7}">
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="B2" sqref="B2:B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1150,12 +1572,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9255F47C-BD46-493C-96D5-2CB6E9A79694}">
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
add account edit functionality
</commit_message>
<xml_diff>
--- a/Accounting App Planning.xlsx
+++ b/Accounting App Planning.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Louise\Documents\GitHub\AccountingApp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{912DEAB8-3CB0-4A9C-913D-7F819AA10B98}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69DA06B2-ACD7-47C1-835D-AC4FB2F6116C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7920" activeTab="1" xr2:uid="{87DFCFEA-2F07-4D1A-89B8-93DFC4EF050B}"/>
   </bookViews>
@@ -663,10 +663,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79F3F73F-D9F7-4B2F-A93D-F7A699778583}">
-  <dimension ref="A1:H24"/>
+  <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G19" sqref="A19:G19"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -679,7 +679,7 @@
     <col min="7" max="7" width="14.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -699,7 +699,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -718,11 +718,11 @@
       <c r="F2" s="1">
         <v>75000</v>
       </c>
-      <c r="H2" t="s">
+      <c r="G2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -742,7 +742,7 @@
         <v>75000</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -762,7 +762,7 @@
         <v>8000</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2</v>
       </c>
@@ -782,7 +782,7 @@
         <v>8000</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>3</v>
       </c>
@@ -802,7 +802,7 @@
         <v>8000</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>3</v>
       </c>
@@ -822,7 +822,7 @@
         <v>8000</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>4</v>
       </c>
@@ -842,7 +842,7 @@
         <v>8000</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>4</v>
       </c>
@@ -862,7 +862,7 @@
         <v>8000</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>6</v>
       </c>
@@ -882,7 +882,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>6</v>
       </c>

</xml_diff>